<commit_message>
Added sensitivity analysis and methods. Needs formatting but works.
</commit_message>
<xml_diff>
--- a/distanceMatrix(2).xlsx
+++ b/distanceMatrix(2).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="15040" yWindow="0" windowWidth="23920" windowHeight="20540" tabRatio="500"/>
+    <workbookView xWindow="8000" yWindow="3720" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="29">
   <si>
     <t>Castle Black</t>
   </si>
@@ -105,10 +105,7 @@
     <t>Checks</t>
   </si>
   <si>
-    <t>decision(1,2,3,4)</t>
-  </si>
-  <si>
-    <t>1,2,3,4,</t>
+    <t>2,3,4,5,6,7,8,10,1213,14,15,16,17</t>
   </si>
 </sst>
 </file>
@@ -171,8 +168,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="69">
+  <cellStyleXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -247,7 +250,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="69">
+  <cellStyles count="75">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -282,6 +285,9 @@
     <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -316,6 +322,9 @@
     <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -647,8 +656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -663,7 +672,7 @@
     <col min="20" max="20" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -680,7 +689,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -700,7 +709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -720,7 +729,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:7">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -740,7 +749,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -760,7 +769,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -779,9 +788,8 @@
       <c r="G6">
         <v>5</v>
       </c>
-      <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:9">
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -800,9 +808,8 @@
       <c r="G7">
         <v>6</v>
       </c>
-      <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:9">
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -821,9 +828,8 @@
       <c r="G8">
         <v>7</v>
       </c>
-      <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="1:9">
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -842,9 +848,8 @@
       <c r="G9">
         <v>8</v>
       </c>
-      <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="1:9">
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
@@ -863,9 +868,8 @@
       <c r="G10">
         <v>9</v>
       </c>
-      <c r="I10" s="2"/>
-    </row>
-    <row r="11" spans="1:9">
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
@@ -884,9 +888,8 @@
       <c r="G11">
         <v>10</v>
       </c>
-      <c r="I11" s="2"/>
-    </row>
-    <row r="12" spans="1:9">
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -905,9 +908,8 @@
       <c r="G12">
         <v>11</v>
       </c>
-      <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="1:9">
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
@@ -926,9 +928,8 @@
       <c r="G13">
         <v>12</v>
       </c>
-      <c r="I13" s="2"/>
-    </row>
-    <row r="14" spans="1:9">
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="2" t="s">
         <v>10</v>
       </c>
@@ -947,9 +948,8 @@
       <c r="G14">
         <v>13</v>
       </c>
-      <c r="I14" s="2"/>
-    </row>
-    <row r="15" spans="1:9">
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" s="2" t="s">
         <v>10</v>
       </c>
@@ -968,9 +968,8 @@
       <c r="G15">
         <v>14</v>
       </c>
-      <c r="I15" s="2"/>
-    </row>
-    <row r="16" spans="1:9">
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
@@ -989,7 +988,6 @@
       <c r="G16">
         <v>15</v>
       </c>
-      <c r="I16" s="2"/>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="2" t="s">
@@ -1010,7 +1008,6 @@
       <c r="G17">
         <v>16</v>
       </c>
-      <c r="I17" s="2"/>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="2" t="s">
@@ -1031,7 +1028,6 @@
       <c r="G18">
         <v>17</v>
       </c>
-      <c r="I18" s="2"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="2" t="s">
@@ -1052,7 +1048,6 @@
       <c r="G19">
         <v>18</v>
       </c>
-      <c r="I19" s="2"/>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="2" t="s">
@@ -1123,12 +1118,6 @@
       <c r="C25">
         <v>390</v>
       </c>
-      <c r="E25" t="s">
-        <v>28</v>
-      </c>
-      <c r="F25" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="2" t="s">
@@ -1150,6 +1139,9 @@
       </c>
       <c r="C27">
         <v>640</v>
+      </c>
+      <c r="E27" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:9">

</xml_diff>